<commit_message>
fix time series fiels
</commit_message>
<xml_diff>
--- a/9-merging/orders_1.xlsx
+++ b/9-merging/orders_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1RvUW3T9bKhn60XFZn1UbUCae90C_xDq2\George Mount - Madecraft\0953 Pandas for Data Analysts  Leveraging Python with Confidence\04_cleaning_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maqimzmnjbt5wavnbicv98tlhog-my.sharepoint.com/personal/george_stringfestanalytics_com/Documents/Stringfest assets/OReilly/oreilly-shortcuts/4-pandas-for-data-analysis/9-merging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2DAB17-1550-437D-A4A8-874ED6161734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{AC2DAB17-1550-437D-A4A8-874ED6161734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09AC8357-D5DE-46A5-B20C-5CEA10B61A8D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{33ADFA24-53B3-4B30-BE3D-799B4789B9D9}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{33ADFA24-53B3-4B30-BE3D-799B4789B9D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,8 +416,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,9 +437,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -476,7 +477,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -582,7 +583,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -724,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -735,19 +736,20 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1484375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -769,11 +771,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>42937</v>
       </c>
       <c r="C2" t="s">
@@ -795,11 +797,11 @@
         <v>17.623199999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>42259</v>
       </c>
       <c r="C3" t="s">
@@ -821,11 +823,11 @@
         <v>12.7746</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>43070</v>
       </c>
       <c r="C4" t="s">
@@ -847,11 +849,11 @@
         <v>7.4824000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>42960</v>
       </c>
       <c r="C5" t="s">
@@ -873,11 +875,11 @@
         <v>4.7969999999999988</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>42300</v>
       </c>
       <c r="C6" t="s">
@@ -899,11 +901,11 @@
         <v>1.1224999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>42992</v>
       </c>
       <c r="C7" t="s">
@@ -925,11 +927,11 @@
         <v>-18.038499999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>42792</v>
       </c>
       <c r="C8" t="s">
@@ -951,11 +953,11 @@
         <v>22.118400000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>42124</v>
       </c>
       <c r="C9" t="s">
@@ -977,11 +979,11 @@
         <v>-15.222500000000011</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>41970</v>
       </c>
       <c r="C10" t="s">
@@ -1003,11 +1005,11 @@
         <v>1.3159999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>42874</v>
       </c>
       <c r="C11" t="s">
@@ -1029,11 +1031,11 @@
         <v>28.176399999999987</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>42688</v>
       </c>
       <c r="C12" t="s">
@@ -1055,11 +1057,11 @@
         <v>-21.717600000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>42677</v>
       </c>
       <c r="C13" t="s">
@@ -1081,11 +1083,11 @@
         <v>15.799199999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>41715</v>
       </c>
       <c r="C14" t="s">
@@ -1107,11 +1109,11 @@
         <v>-447.59469999999988</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>42336</v>
       </c>
       <c r="C15" t="s">
@@ -1133,11 +1135,11 @@
         <v>-19.562399999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A16" t="s">
         <v>39</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>42624</v>
       </c>
       <c r="C16" t="s">
@@ -1159,11 +1161,11 @@
         <v>6.6587999999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A17" t="s">
         <v>41</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>42814</v>
       </c>
       <c r="C17" t="s">
@@ -1185,11 +1187,11 @@
         <v>38.080000000000013</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>41866</v>
       </c>
       <c r="C18" t="s">
@@ -1211,11 +1213,11 @@
         <v>-52.632000000000019</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A19" t="s">
         <v>45</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>43055</v>
       </c>
       <c r="C19" t="s">
@@ -1237,11 +1239,11 @@
         <v>23.987999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
         <v>47</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>42292</v>
       </c>
       <c r="C20" t="s">
@@ -1263,11 +1265,11 @@
         <v>67.991999999999962</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
         <v>49</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>41737</v>
       </c>
       <c r="C21" t="s">
@@ -1289,11 +1291,11 @@
         <v>139.98599999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
         <v>51</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>42614</v>
       </c>
       <c r="C22" t="s">
@@ -1315,11 +1317,11 @@
         <v>206.31600000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A23" t="s">
         <v>53</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>42608</v>
       </c>
       <c r="C23" t="s">
@@ -1341,11 +1343,11 @@
         <v>4.9104000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
         <v>55</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>42924</v>
       </c>
       <c r="C24" t="s">
@@ -1367,11 +1369,11 @@
         <v>8.6729999999999983</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A25" t="s">
         <v>57</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>42068</v>
       </c>
       <c r="C25" t="s">
@@ -1393,11 +1395,11 @@
         <v>-5.4548000000000041</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A26" t="s">
         <v>59</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>42132</v>
       </c>
       <c r="C26" t="s">
@@ -1419,11 +1421,11 @@
         <v>105.83160000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A27" t="s">
         <v>61</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>43042</v>
       </c>
       <c r="C27" t="s">
@@ -1445,11 +1447,11 @@
         <v>27.103200000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A28" t="s">
         <v>63</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>42205</v>
       </c>
       <c r="C28" t="s">
@@ -1471,11 +1473,11 @@
         <v>124.68000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A29" t="s">
         <v>65</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>42605</v>
       </c>
       <c r="C29" t="s">
@@ -1497,11 +1499,11 @@
         <v>-33.319999999999965</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A30" t="s">
         <v>66</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>41958</v>
       </c>
       <c r="C30" t="s">
@@ -1523,11 +1525,11 @@
         <v>146.76929999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A31" t="s">
         <v>68</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>42710</v>
       </c>
       <c r="C31" t="s">
@@ -1549,11 +1551,11 @@
         <v>153.11519999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>42813</v>
       </c>
       <c r="C32" t="s">
@@ -1575,11 +1577,11 @@
         <v>10.949399999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A33" t="s">
         <v>72</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>42633</v>
       </c>
       <c r="C33" t="s">
@@ -1601,11 +1603,11 @@
         <v>37.9848</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A34" t="s">
         <v>74</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>42338</v>
       </c>
       <c r="C34" t="s">
@@ -1627,11 +1629,11 @@
         <v>25.180800000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A35" t="s">
         <v>76</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>42821</v>
       </c>
       <c r="C35" t="s">
@@ -1653,11 +1655,11 @@
         <v>8.1143999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A36" t="s">
         <v>78</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>41850</v>
       </c>
       <c r="C36" t="s">
@@ -1679,11 +1681,11 @@
         <v>259.88959999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A37" t="s">
         <v>80</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>43078</v>
       </c>
       <c r="C37" t="s">
@@ -1705,11 +1707,11 @@
         <v>146.79</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A38" t="s">
         <v>82</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>41911</v>
       </c>
       <c r="C38" t="s">
@@ -1731,11 +1733,11 @@
         <v>-337.80600000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A39" t="s">
         <v>84</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>42736</v>
       </c>
       <c r="C39" t="s">
@@ -1757,11 +1759,11 @@
         <v>-22.684200000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A40" t="s">
         <v>86</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>41791</v>
       </c>
       <c r="C40" t="s">
@@ -1783,11 +1785,11 @@
         <v>41.680000000000007</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A41" t="s">
         <v>88</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>43046</v>
       </c>
       <c r="C41" t="s">
@@ -1809,11 +1811,11 @@
         <v>-140.14079999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A42" t="s">
         <v>90</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>42695</v>
       </c>
       <c r="C42" t="s">
@@ -1835,11 +1837,11 @@
         <v>2.0393999999999934</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A43" t="s">
         <v>92</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>42316</v>
       </c>
       <c r="C43" t="s">
@@ -1861,11 +1863,11 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A44" t="s">
         <v>94</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>42107</v>
       </c>
       <c r="C44" t="s">
@@ -1887,11 +1889,11 @@
         <v>-97.739399999999989</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A45" t="s">
         <v>96</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>43001</v>
       </c>
       <c r="C45" t="s">
@@ -1913,11 +1915,11 @@
         <v>0.59979999999999656</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A46" t="s">
         <v>98</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>42869</v>
       </c>
       <c r="C46" t="s">
@@ -1939,11 +1941,11 @@
         <v>134.99250000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A47" t="s">
         <v>100</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>42612</v>
       </c>
       <c r="C47" t="s">
@@ -1965,11 +1967,11 @@
         <v>3.3889999999999993</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A48" t="s">
         <v>102</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>42980</v>
       </c>
       <c r="C48" t="s">
@@ -1991,11 +1993,11 @@
         <v>-2.6997000000000355</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A49" t="s">
         <v>104</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>42595</v>
       </c>
       <c r="C49" t="s">
@@ -2017,11 +2019,11 @@
         <v>10.7136</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A50" t="s">
         <v>106</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>42959</v>
       </c>
       <c r="C50" t="s">
@@ -2043,11 +2045,11 @@
         <v>92.236799999999988</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A51" t="s">
         <v>108</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>42993</v>
       </c>
       <c r="C51" t="s">
@@ -2069,11 +2071,11 @@
         <v>11.283900000000017</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A52" t="s">
         <v>109</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>42442</v>
       </c>
       <c r="C52" t="s">
@@ -2095,11 +2097,11 @@
         <v>-28.367999999999984</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A53" t="s">
         <v>111</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>41717</v>
       </c>
       <c r="C53" t="s">
@@ -2121,11 +2123,11 @@
         <v>5.5044000000000013</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A54" t="s">
         <v>113</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>42416</v>
       </c>
       <c r="C54" t="s">

</xml_diff>